<commit_message>
added media files for user and item and worked on the html design
</commit_message>
<xml_diff>
--- a/sample_data/item.xlsx
+++ b/sample_data/item.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSDawson\s4\Python\project2\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B2F206-D61E-4AA1-B9F2-E53849FFEEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0EDA9D-4831-45CC-9577-91225F609114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>